<commit_message>
init create dispatch to informal settlement
</commit_message>
<xml_diff>
--- a/lib/registers/LH_Mobile_EFARs.xlsx
+++ b/lib/registers/LH_Mobile_EFARs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="0" windowWidth="28020" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17137,7 +17137,7 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
added mapping of the efars
</commit_message>
<xml_diff>
--- a/lib/registers/LH_Mobile_EFARs.xlsx
+++ b/lib/registers/LH_Mobile_EFARs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="2020" yWindow="20" windowWidth="25600" windowHeight="11180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="97">
   <si>
     <t>Full name</t>
   </si>
@@ -300,12 +300,24 @@
   <si>
     <t xml:space="preserve">No </t>
   </si>
+  <si>
+    <t>Does she live in informal settlement?</t>
+  </si>
+  <si>
+    <t>Informal settlement?</t>
+  </si>
+  <si>
+    <t>Bad address</t>
+  </si>
+  <si>
+    <t>IS?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -345,17 +357,36 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="8"/>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -376,7 +407,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="426">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -387,8 +418,424 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -397,18 +844,437 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="11"/>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="11" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="10"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="10" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="426">
+    <cellStyle name="Bad" xfId="10" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="253" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="255" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="257" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="259" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="261" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="263" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="265" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="267" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="269" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="271" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="273" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="275" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="277" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="279" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="281" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="283" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="285" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="287" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="289" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="291" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="293" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="295" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="297" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="299" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="301" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="303" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="305" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="307" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="309" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="311" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="313" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="315" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="317" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="319" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="321" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="323" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="325" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="327" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="329" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="331" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="333" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="335" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="337" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="339" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="341" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="343" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="345" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="347" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="349" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="351" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="353" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="355" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="357" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="359" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="361" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="363" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="365" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="367" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="369" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="371" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="373" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="375" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="377" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="379" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="381" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="383" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="385" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="387" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="389" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="391" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="393" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="395" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="397" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="399" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="401" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="403" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="405" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="407" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="409" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="411" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="413" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="415" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="417" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="419" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="421" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="423" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="425" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="194" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="196" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="208" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="210" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="212" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="214" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="216" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="218" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="234" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="238" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="242" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="244" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="246" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="248" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="250" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="252" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="254" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="256" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="258" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="260" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="262" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="264" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="266" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="268" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="270" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="272" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="274" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="276" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="278" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="280" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="282" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="284" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="286" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="288" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="290" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="292" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="294" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="296" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="298" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="300" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="302" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="304" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="306" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="308" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="310" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="312" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="314" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="316" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="318" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="320" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="322" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="324" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="326" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="328" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="330" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="332" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="334" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="336" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="338" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="340" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="342" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="344" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="346" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="348" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="350" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="352" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="354" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="356" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="358" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="360" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="362" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="364" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="366" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="368" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="370" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="372" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="374" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="376" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="378" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="380" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="382" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="384" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="386" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="388" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="390" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="392" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="394" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="396" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="398" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="400" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="402" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="404" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="406" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="408" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="410" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="412" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="414" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="416" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="418" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="420" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="422" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="424" builtinId="8" hidden="1"/>
+    <cellStyle name="Neutral" xfId="11" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -17134,10 +18000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -17151,13 +18017,14 @@
     <col min="7" max="7" width="14.6640625" customWidth="1"/>
     <col min="8" max="8" width="15.1640625" customWidth="1"/>
     <col min="9" max="9" width="27.5" customWidth="1"/>
-    <col min="10" max="99" width="12" customWidth="1"/>
+    <col min="10" max="10" width="38.6640625" customWidth="1"/>
+    <col min="11" max="99" width="12" customWidth="1"/>
     <col min="100" max="999" width="13" customWidth="1"/>
     <col min="1000" max="9999" width="14" customWidth="1"/>
     <col min="10000" max="16384" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="51" customHeight="1" thickBot="1">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="51" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -17186,7 +18053,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -17209,7 +18076,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -17232,7 +18099,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -17261,7 +18128,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -17284,27 +18151,31 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
+    <row r="6" spans="1:10" s="4" customFormat="1">
+      <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="4">
         <v>760359761</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H6" t="s">
+      <c r="F6" s="5"/>
+      <c r="H6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="J6" s="4" t="s">
+        <v>93</v>
+      </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -17324,7 +18195,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -17344,47 +18215,55 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
+    <row r="9" spans="1:10" s="4" customFormat="1">
+      <c r="A9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="4">
         <v>840608761</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H9" t="s">
+      <c r="F9" s="5"/>
+      <c r="H9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="J9" s="4" t="s">
+        <v>94</v>
+      </c>
     </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
+    <row r="10" spans="1:10" s="4" customFormat="1">
+      <c r="A10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="4">
         <v>794006561</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H10" t="s">
+      <c r="F10" s="5"/>
+      <c r="H10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="J10" s="4" t="s">
+        <v>95</v>
+      </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -17404,27 +18283,31 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
+    <row r="12" spans="1:10" s="4" customFormat="1">
+      <c r="A12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="4">
         <v>741070062</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H12" t="s">
+      <c r="F12" s="5"/>
+      <c r="H12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="J12" s="4" t="s">
+        <v>96</v>
+      </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -17444,7 +18327,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -17464,7 +18347,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -17484,47 +18367,52 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
-      <c r="A16" t="s">
+    <row r="16" spans="1:10" s="4" customFormat="1">
+      <c r="A16" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="4">
         <v>768847822</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H16" t="s">
+      <c r="F16" s="5"/>
+      <c r="H16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="J16" s="4" t="s">
+        <v>96</v>
+      </c>
     </row>
-    <row r="17" spans="1:9">
-      <c r="A17" t="s">
+    <row r="17" spans="1:10" s="4" customFormat="1">
+      <c r="A17" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="4">
         <v>724198187</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H17" t="s">
+      <c r="F17" s="5"/>
+      <c r="H17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -17544,7 +18432,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -17564,27 +18452,28 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
-      <c r="A20" t="s">
+    <row r="20" spans="1:10" s="4" customFormat="1">
+      <c r="A20" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="4">
         <v>710613241</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H20" t="s">
+      <c r="F20" s="5"/>
+      <c r="H20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -17604,27 +18493,28 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
-      <c r="A22" t="s">
+    <row r="22" spans="1:10" s="6" customFormat="1">
+      <c r="A22" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="6">
         <v>784165728</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H22" t="s">
+      <c r="F22" s="7"/>
+      <c r="H22" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -17644,7 +18534,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>60</v>
       </c>
@@ -17664,7 +18554,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -17684,7 +18574,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -17704,27 +18594,31 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
-      <c r="A27" t="s">
+    <row r="27" spans="1:10" s="6" customFormat="1">
+      <c r="A27" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="6">
         <v>740738972</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H27" t="s">
+      <c r="F27" s="7"/>
+      <c r="H27" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="J27" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
         <v>68</v>
       </c>
@@ -17744,27 +18638,31 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
-      <c r="A29" t="s">
+    <row r="29" spans="1:10" s="4" customFormat="1">
+      <c r="A29" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="4">
         <v>721274964</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H29" t="s">
+      <c r="F29" s="5"/>
+      <c r="H29" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I29" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="J29" s="4" t="s">
+        <v>96</v>
+      </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>72</v>
       </c>
@@ -17784,27 +18682,31 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
-      <c r="A31" t="s">
+    <row r="31" spans="1:10" s="4" customFormat="1">
+      <c r="A31" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="4">
         <v>738733745</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H31" t="s">
+      <c r="F31" s="5"/>
+      <c r="H31" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I31" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="J31" s="4" t="s">
+        <v>96</v>
+      </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
         <v>76</v>
       </c>
@@ -17864,84 +18766,87 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
-      <c r="A35" t="s">
+    <row r="35" spans="1:9" s="4" customFormat="1">
+      <c r="A35" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="4">
         <v>734100446</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H35" t="s">
+      <c r="F35" s="5"/>
+      <c r="H35" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I35" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
-      <c r="A36" t="s">
+    <row r="36" spans="1:9" s="4" customFormat="1">
+      <c r="A36" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="4">
         <v>838865072</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H36" t="s">
+      <c r="F36" s="5"/>
+      <c r="H36" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I36" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
-      <c r="A37" t="s">
+    <row r="37" spans="1:9" s="4" customFormat="1">
+      <c r="A37" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="4">
         <v>844163611</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H37" t="s">
+      <c r="F37" s="5"/>
+      <c r="H37" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I37" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
-      <c r="A38" t="s">
+    <row r="38" spans="1:9" s="4" customFormat="1">
+      <c r="A38" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="4">
         <v>760592632</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" t="s">
+      <c r="D38" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H38" t="s">
+      <c r="F38" s="5"/>
+      <c r="H38" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I38" s="4" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>